<commit_message>
Completed tests through TestProbability_CombinationsWithRepsBigInt_11.
</commit_message>
<xml_diff>
--- a/notes/probability/porbabilityCalcs.xlsx
+++ b/notes/probability/porbabilityCalcs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gowork\src\MikeAustin71\mathopsgo\notes\probability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8F54EB-1490-4C6E-B72A-81D0B86A28D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CB901A-C4DC-4962-A2EE-B35A0F3B5F32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="8535" activeTab="1" xr2:uid="{7421BC9F-5335-4369-A134-12FC8D4251F6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="8535" activeTab="2" xr2:uid="{7421BC9F-5335-4369-A134-12FC8D4251F6}"/>
   </bookViews>
   <sheets>
     <sheet name="CombinationsWithRepeat" sheetId="1" r:id="rId1"/>
     <sheet name="CombinationsWITHOUTRepeat" sheetId="2" r:id="rId2"/>
+    <sheet name="permutationsWITHRepeat" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t xml:space="preserve">         nCr  = </t>
   </si>
@@ -135,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -148,6 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,13 +492,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6840F2-F5F7-4565-BF17-1F825895118D}">
-  <dimension ref="D6:O13"/>
+  <dimension ref="D6:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="6" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
@@ -553,6 +558,26 @@
       </c>
       <c r="M13">
         <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>26</v>
+      </c>
+      <c r="H18" s="6">
+        <f>(FACT(E19+E18-1))/(FACT(+E19)*(FACT(E18-1)))</f>
+        <v>63205303218876.047</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -565,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD93CAA-2890-4AE2-BB2A-1BA493372F6A}">
   <dimension ref="F2:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,4 +666,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D642FE-34F5-45B5-8234-AFA7A2579A9F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored Probability Permutations with repetitions. Ordered sampling with replacement.
</commit_message>
<xml_diff>
--- a/notes/probability/porbabilityCalcs.xlsx
+++ b/notes/probability/porbabilityCalcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gowork\src\MikeAustin71\mathopsgo\notes\probability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CB901A-C4DC-4962-A2EE-B35A0F3B5F32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BF6392-4677-4EBC-A288-632B565BDA33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="8535" activeTab="2" xr2:uid="{7421BC9F-5335-4369-A134-12FC8D4251F6}"/>
   </bookViews>
@@ -672,7 +672,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D642FE-34F5-45B5-8234-AFA7A2579A9F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>